<commit_message>
Updates to weather-related code
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeyerCarter\Documents\Comp-Sci-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E30080-11F3-43EF-B3F8-CECDF2351E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75404CD8-8A01-4782-A309-D8CC04D1DAD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{900EE39F-17EC-44C3-BE32-FFBEBC0E6A72}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{900EE39F-17EC-44C3-BE32-FFBEBC0E6A72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAF1C6D-A6B7-405C-940B-7B95F136D7C4}">
   <dimension ref="B2:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B30" zoomScale="306" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="306" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -775,7 +775,7 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D28" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Added Solder connections for wifi
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PedersonJosh\GitHub\Research\Comp-Sci-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260F7B3E-14B5-4C20-BA09-423773A01D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6527F66C-7A5B-4511-9864-918AC4C54823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{900EE39F-17EC-44C3-BE32-FFBEBC0E6A72}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
   <si>
     <t>Pin</t>
   </si>
@@ -228,6 +228,18 @@
   </si>
   <si>
     <t>D2</t>
+  </si>
+  <si>
+    <t>5v and EN</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Yellow Taped Bundle</t>
+  </si>
+  <si>
+    <t>Non Taped</t>
   </si>
 </sst>
 </file>
@@ -579,17 +591,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAF1C6D-A6B7-405C-940B-7B95F136D7C4}">
-  <dimension ref="B2:F50"/>
+  <dimension ref="B2:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="145" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="145" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="35.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
@@ -700,7 +713,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>60</v>
       </c>
@@ -711,7 +724,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
         <v>23</v>
       </c>
@@ -725,7 +738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>61</v>
       </c>
@@ -736,7 +749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>26</v>
       </c>
@@ -744,7 +757,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>28</v>
       </c>
@@ -755,7 +768,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>30</v>
       </c>
@@ -763,7 +776,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>31</v>
       </c>
@@ -774,7 +787,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>23</v>
       </c>
@@ -782,7 +795,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>30</v>
       </c>
@@ -790,7 +803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>26</v>
       </c>
@@ -798,7 +811,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>34</v>
       </c>
@@ -808,40 +821,94 @@
       <c r="D30" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
         <v>6</v>
       </c>
       <c r="D31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" t="s">
+        <v>30</v>
+      </c>
+      <c r="H31" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
         <v>36</v>
       </c>
       <c r="D32" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E32" t="s">
+        <v>23</v>
+      </c>
+      <c r="F32" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" t="s">
+        <v>23</v>
+      </c>
+      <c r="H32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
         <v>37</v>
       </c>
       <c r="D33" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F33" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
         <v>38</v>
       </c>
       <c r="D34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>65</v>
+      </c>
+      <c r="F34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
         <v>39</v>
       </c>
@@ -849,7 +916,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
         <v>40</v>
       </c>
@@ -857,7 +924,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
         <v>41</v>
       </c>
@@ -865,7 +932,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
         <v>42</v>
       </c>
@@ -873,12 +940,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>51</v>
       </c>
@@ -889,7 +956,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
         <v>6</v>
       </c>
@@ -897,7 +964,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
         <v>49</v>
       </c>
@@ -905,7 +972,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
         <v>50</v>
       </c>
@@ -913,7 +980,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>54</v>
       </c>
@@ -924,7 +991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
         <v>6</v>
       </c>
@@ -932,7 +999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
         <v>55</v>
       </c>
@@ -940,7 +1007,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
Added Unzipped Library folder
</commit_message>
<xml_diff>
--- a/Pins.xlsx
+++ b/Pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PedersonJosh\GitHub\Research\Comp-Sci-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6501F38-4098-4ABC-8510-023D101D4E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56F7180-08D7-4A64-AF9E-ACF726DDA8E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{900EE39F-17EC-44C3-BE32-FFBEBC0E6A72}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="72">
   <si>
     <t>Pin</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Green</t>
   </si>
   <si>
-    <t>Read</t>
-  </si>
-  <si>
     <t>Blue  (dataPin)</t>
   </si>
   <si>
@@ -246,6 +243,15 @@
   </si>
   <si>
     <t>pin</t>
+  </si>
+  <si>
+    <t>Female order</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>black</t>
   </si>
 </sst>
 </file>
@@ -613,13 +619,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAF1C6D-A6B7-405C-940B-7B95F136D7C4}">
   <dimension ref="B2:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E20" zoomScale="145" zoomScaleNormal="240" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="145" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" customWidth="1"/>
@@ -627,7 +633,7 @@
     <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>2</v>
       </c>
@@ -638,7 +644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -649,7 +655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>6</v>
       </c>
@@ -657,7 +663,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>7</v>
       </c>
@@ -665,7 +671,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -673,7 +679,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -684,7 +690,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -692,7 +698,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>14</v>
       </c>
@@ -700,44 +706,73 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>16</v>
       </c>
       <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="D13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
+      <c r="D15" t="s">
         <v>19</v>
       </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" t="s">
-        <v>22</v>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -748,24 +783,24 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
         <v>23</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" t="s">
         <v>24</v>
-      </c>
-      <c r="E18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
@@ -773,26 +808,26 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" t="s">
         <v>6</v>
@@ -800,18 +835,18 @@
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
@@ -819,7 +854,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" t="s">
         <v>6</v>
@@ -827,39 +862,39 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" t="s">
         <v>34</v>
-      </c>
-      <c r="C30" t="s">
-        <v>35</v>
       </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
       <c r="E30" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G30" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30" t="s">
         <v>65</v>
       </c>
-      <c r="F30" t="s">
-        <v>69</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="I30" t="s">
         <v>68</v>
       </c>
-      <c r="H30" t="s">
-        <v>66</v>
-      </c>
-      <c r="I30" t="s">
-        <v>69</v>
-      </c>
       <c r="J30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.3">
@@ -870,113 +905,113 @@
         <v>6</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="D32" t="s">
-        <v>43</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H32" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J33" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D33" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" t="s">
+        <v>44</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J34" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D34" t="s">
-        <v>45</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D36" t="s">
         <v>5</v>
@@ -984,31 +1019,31 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="D39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
         <v>5</v>
@@ -1024,23 +1059,23 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1059,34 +1094,34 @@
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D49" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>